<commit_message>
HW: Version 2.0 Layout, BOM, Gerber-files created
</commit_message>
<xml_diff>
--- a/Electronic/Production/BOM/BOM_ZumoComSystem.xlsx
+++ b/Electronic/Production/BOM/BOM_ZumoComSystem.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nschneider\Documents\NT_Projekte\ZumoCom\Repository\Electronic\Production\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D78D8E1-5BD9-4AEB-823C-588A3101A13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6BC83C-A3FF-437A-A140-4B5EC36030F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="222">
   <si>
     <t>ZumoComSystem</t>
   </si>
@@ -42,9 +42,6 @@
     <t>MF-USML450/12-2</t>
   </si>
   <si>
-    <t>C2012X5R1V106M085AC</t>
-  </si>
-  <si>
     <t>C3216X5R1V226M160AC</t>
   </si>
   <si>
@@ -72,27 +69,9 @@
     <t>Battery_Cell</t>
   </si>
   <si>
-    <t xml:space="preserve">    C4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    C5</t>
-  </si>
-  <si>
     <t>C0805C274K5RACTU</t>
   </si>
   <si>
-    <t>&gt;  C7, C8</t>
-  </si>
-  <si>
-    <t>18p</t>
-  </si>
-  <si>
-    <t>C0603C180J5GAC7867</t>
-  </si>
-  <si>
-    <t>&gt;  C9, C10, C12, C13</t>
-  </si>
-  <si>
     <t>100n</t>
   </si>
   <si>
@@ -102,42 +81,18 @@
     <t>CC0603JRX7R9BB104</t>
   </si>
   <si>
-    <t xml:space="preserve">    C11</t>
-  </si>
-  <si>
     <t>1u</t>
   </si>
   <si>
     <t>C1608X5R1H105M080AB</t>
   </si>
   <si>
-    <t xml:space="preserve">    C14</t>
-  </si>
-  <si>
-    <t>4.7u</t>
-  </si>
-  <si>
-    <t>C1608X5R1V475M080AC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    C15</t>
-  </si>
-  <si>
     <t>330n</t>
   </si>
   <si>
     <t>C1608X5R1H334M080AB</t>
   </si>
   <si>
-    <t>&gt;  C16-C18</t>
-  </si>
-  <si>
-    <t>10n</t>
-  </si>
-  <si>
-    <t>C0603C103M5RAC7411</t>
-  </si>
-  <si>
     <t xml:space="preserve">    D1</t>
   </si>
   <si>
@@ -162,18 +117,12 @@
     <t>P6SMB10A-E3/52</t>
   </si>
   <si>
-    <t>&gt;  D4-D6</t>
-  </si>
-  <si>
     <t>D5V0S1U2WS-7</t>
   </si>
   <si>
     <t>Diodes Incorporated</t>
   </si>
   <si>
-    <t xml:space="preserve">    D7</t>
-  </si>
-  <si>
     <t>LED, red</t>
   </si>
   <si>
@@ -195,9 +144,6 @@
     <t xml:space="preserve">    D10</t>
   </si>
   <si>
-    <t>LED_RGBA</t>
-  </si>
-  <si>
     <t>Broadcom Limited</t>
   </si>
   <si>
@@ -219,15 +165,6 @@
     <t>Molex</t>
   </si>
   <si>
-    <t xml:space="preserve">    J2</t>
-  </si>
-  <si>
-    <t>66200221122</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    J3</t>
-  </si>
-  <si>
     <t>USB_B_Micro</t>
   </si>
   <si>
@@ -255,9 +192,6 @@
     <t xml:space="preserve">    L1</t>
   </si>
   <si>
-    <t xml:space="preserve">    L2</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Q1</t>
   </si>
   <si>
@@ -270,9 +204,6 @@
     <t>RQ5E065AJTCL</t>
   </si>
   <si>
-    <t>&gt;  Q4, Q5</t>
-  </si>
-  <si>
     <t>NPN-SS8050</t>
   </si>
   <si>
@@ -300,9 +231,6 @@
     <t>RC0603FR-070RL</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -315,9 +243,6 @@
     <t>CRGCQ0603F470R</t>
   </si>
   <si>
-    <t xml:space="preserve">    R9</t>
-  </si>
-  <si>
     <t>2k</t>
   </si>
   <si>
@@ -330,12 +255,6 @@
     <t>CRGCQ0603F12K</t>
   </si>
   <si>
-    <t>4.7k</t>
-  </si>
-  <si>
-    <t>RC0603FR-074K7L</t>
-  </si>
-  <si>
     <t>4.93k / 0.1%</t>
   </si>
   <si>
@@ -354,18 +273,9 @@
     <t xml:space="preserve">MLL1200S </t>
   </si>
   <si>
-    <t xml:space="preserve">    SW2</t>
-  </si>
-  <si>
-    <t>RESET_AP-Mode</t>
-  </si>
-  <si>
     <t>TL3342F260QG</t>
   </si>
   <si>
-    <t>&gt;  SW3-SW5</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U1</t>
   </si>
   <si>
@@ -381,45 +291,12 @@
     <t xml:space="preserve">    U3</t>
   </si>
   <si>
-    <t>MAX3421EEHJ+T</t>
-  </si>
-  <si>
-    <t>Maxim Integrated</t>
-  </si>
-  <si>
     <t xml:space="preserve">    U4</t>
   </si>
   <si>
     <t>S-8252AAL-M6T1U</t>
   </si>
   <si>
-    <t>ablic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U5</t>
-  </si>
-  <si>
-    <t>CP2102</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CP2102N-A02-GQFN28 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESP32-WROOM-32D-N16 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    Y1</t>
-  </si>
-  <si>
-    <t>FL1200112_12MHz</t>
-  </si>
-  <si>
-    <t>FL1200112</t>
-  </si>
-  <si>
     <t>&gt;  BT1, BT2</t>
   </si>
   <si>
@@ -459,66 +336,18 @@
     <t xml:space="preserve">    BT1*,BT2*</t>
   </si>
   <si>
-    <t>ADP2371ACPZ-3.3-R7</t>
-  </si>
-  <si>
-    <t>Coilcraft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">XAL4030-682MEC </t>
-  </si>
-  <si>
     <t>GRM31CC81E226KE11L</t>
   </si>
   <si>
-    <t xml:space="preserve">    C1</t>
-  </si>
-  <si>
-    <t>&gt;  C2, C6</t>
-  </si>
-  <si>
     <t>10u</t>
   </si>
   <si>
-    <t xml:space="preserve">    C3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Keystone Electronics </t>
-  </si>
-  <si>
     <t xml:space="preserve"> Murata Electronics </t>
   </si>
   <si>
-    <t>6.8u</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R5</t>
-  </si>
-  <si>
-    <t>&gt;  R6, R16</t>
-  </si>
-  <si>
-    <t>&gt;  R7, R8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R10</t>
-  </si>
-  <si>
-    <t>&gt;  R11, R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R13</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R19</t>
   </si>
   <si>
-    <t>KMR221GLFS</t>
-  </si>
-  <si>
-    <t>ADP2370ACPZ-3.3-R7</t>
-  </si>
-  <si>
     <t>22u</t>
   </si>
   <si>
@@ -531,21 +360,6 @@
     <t>100u</t>
   </si>
   <si>
-    <t>Schottky (3V3,VDD)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microchip Technology / Atmel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LSM115JE3/TR13 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">    D11</t>
-  </si>
-  <si>
-    <t>&gt;  J4, J6</t>
-  </si>
-  <si>
     <t>Pin-Header 2x13</t>
   </si>
   <si>
@@ -567,30 +381,15 @@
     <t xml:space="preserve">TSM260P02CX RFG </t>
   </si>
   <si>
-    <t>&gt;  R2, R3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    R18</t>
-  </si>
-  <si>
     <t>10k / 0.1%</t>
   </si>
   <si>
-    <t>&gt;  TP1, TP2</t>
-  </si>
-  <si>
     <t>TP_2P</t>
   </si>
   <si>
     <t xml:space="preserve">   J4*, J6*</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0603JR-1322RL </t>
-  </si>
-  <si>
     <t>Pin-Socket 2x13 for Zumo Robot</t>
   </si>
   <si>
@@ -600,27 +399,12 @@
     <t>LED, yellow</t>
   </si>
   <si>
-    <t xml:space="preserve">    JP1</t>
-  </si>
-  <si>
-    <t>Jumper_3_Bridged12</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Q7</t>
   </si>
   <si>
-    <t>&gt;  R1, R14, R15, R17, R20, R27, R30-R32</t>
-  </si>
-  <si>
     <t xml:space="preserve">    R21</t>
   </si>
   <si>
-    <t>&gt;  R22, R23</t>
-  </si>
-  <si>
-    <t>&gt;  R24-R26</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Kyocera AVX </t>
   </si>
   <si>
@@ -630,34 +414,283 @@
     <t xml:space="preserve">150060YS55040 </t>
   </si>
   <si>
-    <t xml:space="preserve"> Würth Elektronik </t>
-  </si>
-  <si>
     <t>RT0603FRE07100RL</t>
   </si>
   <si>
     <t>Bourns</t>
   </si>
   <si>
-    <t xml:space="preserve"> CR0603-FX-6200ELF </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> C&amp;K</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Silicon Labs </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Espressif Systems</t>
-  </si>
-  <si>
-    <t>TSW-107-09-T-D</t>
-  </si>
-  <si>
-    <t>V1.2</t>
-  </si>
-  <si>
     <t>Revison:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keystone Electronics </t>
+  </si>
+  <si>
+    <t>&gt;  C1, C3, C4</t>
+  </si>
+  <si>
+    <t>&gt;  C2, C5, C7</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL31A106KBHNNNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C10</t>
+  </si>
+  <si>
+    <t>&gt;  C11, C14</t>
+  </si>
+  <si>
+    <t>Kemet</t>
+  </si>
+  <si>
+    <t>T491A106K020AT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    C13</t>
+  </si>
+  <si>
+    <t>LED_ARGB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D4</t>
+  </si>
+  <si>
+    <t>&gt;  D5-D7, D11-D13</t>
+  </si>
+  <si>
+    <t>40V/2A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ROHM Semiconductor </t>
+  </si>
+  <si>
+    <t>RBR2LAM40ATFTR</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>SML-D12D1WT86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    D16</t>
+  </si>
+  <si>
+    <t>1N5819HW1-7-F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    IC1</t>
+  </si>
+  <si>
+    <t>ABLIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    IC2</t>
+  </si>
+  <si>
+    <t>MCP73844-840I_MS</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>MCP73844T-840I/MS</t>
+  </si>
+  <si>
+    <t>&gt;  J2, J3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    J4</t>
+  </si>
+  <si>
+    <t>TSW-107-07-T-D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    J6</t>
+  </si>
+  <si>
+    <t>PJ-090BH</t>
+  </si>
+  <si>
+    <t>CUI Devices</t>
+  </si>
+  <si>
+    <t>&gt;  JP1, JP2</t>
+  </si>
+  <si>
+    <t>SolderJumper_2_Open</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Q4</t>
+  </si>
+  <si>
+    <t>Q_PMOS_GSD</t>
+  </si>
+  <si>
+    <t>Taiwan Semiconductor Corporation</t>
+  </si>
+  <si>
+    <t>TSM500P02CX RFG</t>
+  </si>
+  <si>
+    <t>&gt;  Q5, Q6</t>
+  </si>
+  <si>
+    <t>&gt;  R1, R5, R6, R10, R11, R14, R15, R31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R2</t>
+  </si>
+  <si>
+    <t>&gt;  R3, R4</t>
+  </si>
+  <si>
+    <t>&gt;  R7-R9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CR0603-FX-6200ELF </t>
+  </si>
+  <si>
+    <t>&gt;  R12, R13, R18</t>
+  </si>
+  <si>
+    <t>&gt;  R16, R17</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RMCF0603FT100K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R20</t>
+  </si>
+  <si>
+    <t>220m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERJ-6RQFR22V </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R25</t>
+  </si>
+  <si>
+    <t>&gt;  R26, R27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R28</t>
+  </si>
+  <si>
+    <t>22.1k / 0.1%</t>
+  </si>
+  <si>
+    <t>KOA Speer</t>
+  </si>
+  <si>
+    <t>RN73H1JTTD2212B25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R29</t>
+  </si>
+  <si>
+    <t>47.5k / 0.5%</t>
+  </si>
+  <si>
+    <t>RN73H1JTTD4752D50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    R30</t>
+  </si>
+  <si>
+    <t>1k</t>
+  </si>
+  <si>
+    <t>Vishay / Draloric</t>
+  </si>
+  <si>
+    <t>RCA04021K00JNED</t>
+  </si>
+  <si>
+    <t>User_Button</t>
+  </si>
+  <si>
+    <t>&gt;  SW2-SW5</t>
+  </si>
+  <si>
+    <t>SW_Push</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Omron Electronics </t>
+  </si>
+  <si>
+    <t>B3U-1000P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    SW6</t>
+  </si>
+  <si>
+    <t>&gt;  TP1-TP4</t>
+  </si>
+  <si>
+    <t>TestPoint</t>
+  </si>
+  <si>
+    <t>&gt;  TP5, TP7</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>espressif</t>
+  </si>
+  <si>
+    <t>CP2102N-Axx-xQFN28</t>
+  </si>
+  <si>
+    <t>Silicon Laboratories Inc.</t>
+  </si>
+  <si>
+    <t>LM1117MP-3.3</t>
+  </si>
+  <si>
+    <t>v2.0</t>
   </si>
 </sst>
 </file>
@@ -774,8 +807,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A4:E70" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A4:E70" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabelle1" displayName="Tabelle1" ref="A4:E72" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="A4:E72" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Reference" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="3"/>
@@ -1050,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:H74"/>
+  <dimension ref="A2:H76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,10 +1108,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>210</v>
+        <v>131</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.35">
@@ -1086,30 +1119,30 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>134</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>140</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>131</v>
+        <v>90</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>152</v>
+        <v>132</v>
       </c>
       <c r="D5" s="3">
         <v>1043</v>
@@ -1120,52 +1153,52 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>164</v>
+        <v>15</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>153</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>150</v>
+        <v>104</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>135</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>5</v>
+        <v>136</v>
       </c>
       <c r="E7" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>165</v>
+        <v>20</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -1174,16 +1207,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>15</v>
+        <v>138</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>166</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
@@ -1192,16 +1225,16 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>139</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>167</v>
+        <v>107</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>105</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="E10" s="5">
         <v>1</v>
@@ -1210,52 +1243,52 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>140</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>108</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="E11" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>142</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>24</v>
+        <v>143</v>
       </c>
       <c r="E12" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>25</v>
+        <v>144</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="E13" s="5">
         <v>1</v>
@@ -1264,16 +1297,16 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>28</v>
+        <v>145</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>29</v>
+        <v>110</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="E14" s="5">
         <v>1</v>
@@ -1282,16 +1315,16 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>32</v>
+        <v>146</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E15" s="5">
         <v>1</v>
@@ -1300,34 +1333,34 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>123</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>9</v>
+        <v>127</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>36</v>
+        <v>128</v>
       </c>
       <c r="E16" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>198</v>
+        <v>127</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="E17" s="5">
         <v>1</v>
@@ -1336,16 +1369,16 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>147</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>39</v>
+        <v>127</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E18" s="5">
         <v>1</v>
@@ -1354,52 +1387,52 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>41</v>
+        <v>148</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="E19" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="H19" s="2"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>46</v>
+        <v>149</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>47</v>
+        <v>150</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>46</v>
+        <v>151</v>
       </c>
       <c r="E20" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="2"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>169</v>
+        <v>56</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
       <c r="E21" s="5">
         <v>1</v>
@@ -1408,16 +1441,16 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>190</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>200</v>
+        <v>29</v>
       </c>
       <c r="E22" s="5">
         <v>1</v>
@@ -1426,16 +1459,16 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>53</v>
+        <v>9</v>
       </c>
       <c r="E23" s="5">
         <v>1</v>
@@ -1444,16 +1477,16 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>55</v>
+        <v>155</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>199</v>
+        <v>24</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E24" s="5">
         <v>1</v>
@@ -1462,16 +1495,16 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>171</v>
+        <v>156</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>56</v>
+        <v>157</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="E25" s="5">
         <v>1</v>
@@ -1480,10 +1513,10 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>2</v>
@@ -1498,16 +1531,16 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>61</v>
+        <v>158</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="E27" s="5">
         <v>1</v>
@@ -1516,16 +1549,16 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>64</v>
+        <v>160</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>65</v>
+        <v>163</v>
       </c>
       <c r="E28" s="5">
         <v>1</v>
@@ -1534,16 +1567,16 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="E29" s="5">
         <v>1</v>
@@ -1552,16 +1585,16 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>173</v>
+        <v>111</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E30" s="5">
         <v>2</v>
@@ -1570,16 +1603,16 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>71</v>
+        <v>165</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>208</v>
+        <v>166</v>
       </c>
       <c r="E31" s="5">
         <v>1</v>
@@ -1588,16 +1621,16 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="E32" s="5">
         <v>1</v>
@@ -1606,16 +1639,16 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>192</v>
+        <v>168</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>92</v>
+        <v>169</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
       <c r="E33" s="5">
         <v>1</v>
@@ -1624,16 +1657,16 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>154</v>
+        <v>46</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>146</v>
+        <v>47</v>
       </c>
       <c r="E34" s="5">
         <v>1</v>
@@ -1642,34 +1675,34 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>76</v>
+        <v>170</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>175</v>
+        <v>68</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>176</v>
+        <v>68</v>
       </c>
       <c r="E35" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="2"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>77</v>
+        <v>54</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>177</v>
+        <v>112</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>178</v>
+        <v>113</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>179</v>
+        <v>114</v>
       </c>
       <c r="E36" s="5">
         <v>1</v>
@@ -1677,34 +1710,34 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="E37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H37" s="2"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="E38" s="5">
         <v>2</v>
@@ -1713,16 +1746,16 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>193</v>
+        <v>172</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>85</v>
+        <v>173</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>86</v>
+        <v>174</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>85</v>
+        <v>175</v>
       </c>
       <c r="E39" s="5">
         <v>1</v>
@@ -1730,67 +1763,67 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>89</v>
+        <v>61</v>
       </c>
       <c r="E40" s="5">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="B41" s="3">
-        <v>22</v>
+        <v>124</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>115</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>23</v>
+        <v>116</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>187</v>
+        <v>117</v>
       </c>
       <c r="E41" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="B42" s="3">
-        <v>0</v>
+        <v>177</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="E42" s="5">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>91</v>
+        <v>178</v>
+      </c>
+      <c r="B43" s="3">
+        <v>300</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="E43" s="5">
         <v>1</v>
@@ -1798,16 +1831,16 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>179</v>
+      </c>
+      <c r="B44" s="3">
+        <v>100</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
       <c r="E44" s="5">
         <v>2</v>
@@ -1815,84 +1848,84 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>157</v>
+        <v>180</v>
       </c>
       <c r="B45" s="3">
-        <v>470</v>
+        <v>620</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>88</v>
+        <v>130</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="E45" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>96</v>
+        <v>182</v>
       </c>
       <c r="B46" s="3">
         <v>0</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>139</v>
+        <v>67</v>
       </c>
       <c r="E46" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>97</v>
+        <v>183</v>
+      </c>
+      <c r="B47" s="3">
+        <v>470</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>23</v>
+        <v>65</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="E47" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>99</v>
+        <v>184</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>88</v>
+        <v>185</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>100</v>
+        <v>186</v>
       </c>
       <c r="E48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>160</v>
+        <v>187</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>101</v>
+        <v>188</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>23</v>
+        <v>189</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>102</v>
+        <v>190</v>
       </c>
       <c r="E49" s="5">
         <v>1</v>
@@ -1900,16 +1933,16 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>183</v>
+        <v>125</v>
+      </c>
+      <c r="B50" s="3">
+        <v>0</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>88</v>
+        <v>16</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E50" s="5">
         <v>1</v>
@@ -1917,16 +1950,16 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="E51" s="5">
         <v>1</v>
@@ -1934,16 +1967,16 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="B52" s="3">
-        <v>300</v>
+        <v>192</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>2</v>
+        <v>65</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
       <c r="E52" s="5">
         <v>1</v>
@@ -1951,67 +1984,67 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>196</v>
-      </c>
-      <c r="B53" s="3">
-        <v>100</v>
+        <v>193</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>202</v>
+        <v>77</v>
       </c>
       <c r="E53" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B54" s="3">
-        <v>620</v>
+        <v>194</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>204</v>
+        <v>70</v>
       </c>
       <c r="E54" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>106</v>
+        <v>195</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>1</v>
+        <v>74</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="E55" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>109</v>
+        <v>196</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>110</v>
+        <v>197</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>3</v>
+        <v>198</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>111</v>
+        <v>199</v>
       </c>
       <c r="E56" s="5">
         <v>1</v>
@@ -2019,50 +2052,50 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>112</v>
+        <v>200</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>162</v>
+        <v>201</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>162</v>
+        <v>202</v>
       </c>
       <c r="E57" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>184</v>
+        <v>203</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>185</v>
+        <v>204</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>92</v>
+        <v>205</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>92</v>
+        <v>206</v>
       </c>
       <c r="E58" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>113</v>
+        <v>79</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>114</v>
+        <v>207</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>115</v>
+        <v>3</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="E59" s="5">
         <v>1</v>
@@ -2070,33 +2103,33 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>116</v>
+        <v>208</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>163</v>
+        <v>209</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>115</v>
+        <v>210</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>144</v>
+        <v>211</v>
       </c>
       <c r="E60" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>117</v>
+        <v>212</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="E61" s="5">
         <v>1</v>
@@ -2104,50 +2137,50 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>120</v>
+        <v>213</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>121</v>
+        <v>214</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>122</v>
+        <v>68</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>121</v>
+        <v>68</v>
       </c>
       <c r="E62" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>123</v>
+        <v>215</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>206</v>
+        <v>68</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
       <c r="E63" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>127</v>
+        <v>216</v>
       </c>
       <c r="E64" s="5">
         <v>1</v>
@@ -2155,91 +2188,125 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>86</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>129</v>
+        <v>218</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>47</v>
+        <v>219</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>130</v>
+        <v>218</v>
       </c>
       <c r="E65" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="A66" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E66" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>141</v>
+        <v>220</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D67" s="3">
-        <v>100833</v>
+        <v>68</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="E67" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="E68" s="5">
-        <v>1</v>
-      </c>
+      <c r="A68" s="3"/>
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>186</v>
+        <v>102</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>188</v>
+        <v>100</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>189</v>
+        <v>101</v>
+      </c>
+      <c r="D69" s="3">
+        <v>100833</v>
       </c>
       <c r="E69" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D73" s="3"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="3"/>
-      <c r="B74" s="3"/>
-      <c r="C74" s="3"/>
+      <c r="A70" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E71" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>